<commit_message>
Adding instantiation of attack gameobjects
</commit_message>
<xml_diff>
--- a/ProjectApopalypse_Unity/Excel/Attacks.xlsx
+++ b/ProjectApopalypse_Unity/Excel/Attacks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectApopalypse\ProjectApopalypse_Unity\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61D67D7-DB79-45D9-A9EF-2FFA20EB1B2B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40B26C1-7445-420D-B511-BC351EF7441E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{3A2312A1-F630-46F4-AF7A-37D6220B2126}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>technicalName</t>
   </si>
@@ -37,12 +37,6 @@
   </si>
   <si>
     <t>Default Attack</t>
-  </si>
-  <si>
-    <t>attackInt</t>
-  </si>
-  <si>
-    <t>attackBool</t>
   </si>
 </sst>
 </file>
@@ -402,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D66FF625-BC64-4C5F-8916-6942D597EF48}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="7.8" x14ac:dyDescent="0.15"/>
@@ -415,32 +409,20 @@
     <col min="3" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" s="1">
-        <v>95</v>
-      </c>
-      <c r="D2" s="1" t="b">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deciding to remove the attack data sheet in favour of having all the data in the unit file
</commit_message>
<xml_diff>
--- a/ProjectApopalypse_Unity/Excel/Attacks.xlsx
+++ b/ProjectApopalypse_Unity/Excel/Attacks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectApopalypse\ProjectApopalypse_Unity\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5539C888-669A-47AB-9044-A988813A1A07}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9951CAB-CF21-4B89-B7A5-8D9CE09BE040}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{3A2312A1-F630-46F4-AF7A-37D6220B2126}"/>
   </bookViews>
@@ -402,14 +402,15 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="7.8" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="8.77734375" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="44.33203125" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">

</xml_diff>